<commit_message>
validatieregel toegevoegd (t.b.v. Regelingsgebied)
</commit_message>
<xml_diff>
--- a/1.0_ow-1.0.1_op-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.12.xlsx
+++ b/1.0_ow-1.0.1_op-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\1.0_ow-1.0.1_op-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB121A02-E6A1-4F19-91BA-8CA8CD3814F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F88C78-3702-437F-A358-3179B2C028A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2411" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="239">
   <si>
     <t>Beschrijving</t>
   </si>
@@ -749,13 +749,19 @@
   </si>
   <si>
     <t>Indien de normwaarde van het type 'waardeInRegeltekst' is, mag er maar één normwaarde voorkomen.</t>
+  </si>
+  <si>
+    <t>TPOD2180</t>
+  </si>
+  <si>
+    <t>Per Regeling moet er een Regelingsgebied zijn aangeleverd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -802,6 +808,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1024,11 +1048,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1124,10 +1152,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{D101CD80-1AD3-420D-BF6F-E7982F1FE2DE}"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{DD73F50D-CE68-4CBD-BD67-3376699AD112}"/>
+    <cellStyle name="Standaard 3" xfId="3" xr:uid="{C5095CC6-E89F-4BD7-837D-4477A4D268A5}"/>
+    <cellStyle name="Standaard 3 2" xfId="4" xr:uid="{3336DED5-B670-47A9-81F8-E0384FA2DDCF}"/>
+    <cellStyle name="Standaard 4" xfId="2" xr:uid="{09E6B307-1DDA-4AD9-8A57-F14FEA913823}"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -9150,7 +9209,81 @@
       <c r="AB93" s="29"/>
     </row>
     <row r="94" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="Y94" s="29"/>
+      <c r="A94" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="B94" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="C94" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="D94" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E94" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F94" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G94" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H94" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="I94" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="J94" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="K94" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="L94" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="M94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="N94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="P94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="R94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="S94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="T94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="U94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="V94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="W94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="X94" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y94" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="Z94" s="30"/>
       <c r="AA94" s="29"/>
       <c r="AB94" s="29"/>

</xml_diff>

<commit_message>
Excel-bestand aangepast (twee nieuwe validatieregels van manifest-OW)
</commit_message>
<xml_diff>
--- a/1.0_ow-1.0.1_op-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.12.xlsx
+++ b/1.0_ow-1.0.1_op-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\1.0_ow-1.0.1_op-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F88C78-3702-437F-A358-3179B2C028A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33266E60-30C7-40B3-A471-93B8EB055580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="1812" yWindow="1332" windowWidth="18552" windowHeight="11028" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TPOD-werkversieBert" sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2486" uniqueCount="243">
   <si>
     <t>Beschrijving</t>
   </si>
@@ -755,6 +755,18 @@
   </si>
   <si>
     <t>Per Regeling moet er een Regelingsgebied zijn aangeleverd.</t>
+  </si>
+  <si>
+    <t>TPOD2190</t>
+  </si>
+  <si>
+    <t>In het manifest-OW mag het objecttype Geometrie niet voorkomen.</t>
+  </si>
+  <si>
+    <t>In het manifest-OW mag een bestandsnaam niet eindigen op '.gml'</t>
+  </si>
+  <si>
+    <t>TPOD2200</t>
   </si>
 </sst>
 </file>
@@ -1669,11 +1681,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796636CA-F9C3-46BC-98AE-E8485AAD557E}">
-  <dimension ref="A1:AB117"/>
+  <dimension ref="A1:AB116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9289,13 +9301,161 @@
       <c r="AB94" s="29"/>
     </row>
     <row r="95" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="Y95" s="29"/>
+      <c r="A95" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="B95" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="C95" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D95" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E95" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F95" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G95" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H95" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="I95" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="J95" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="K95" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="L95" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="M95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="N95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="P95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="R95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="S95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="T95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="U95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="V95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="W95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="X95" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y95" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="Z95" s="30"/>
       <c r="AA95" s="29"/>
       <c r="AB95" s="29"/>
     </row>
     <row r="96" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="Y96" s="29"/>
+      <c r="A96" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="B96" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="C96" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="D96" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E96" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F96" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G96" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H96" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="I96" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="J96" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="K96" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="L96" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="M96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="N96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="P96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="R96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="S96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="T96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="U96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="V96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="W96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="X96" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y96" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="Z96" s="30"/>
       <c r="AA96" s="29"/>
       <c r="AB96" s="29"/>
@@ -9408,9 +9568,9 @@
       <c r="AA114" s="29"/>
       <c r="AB114" s="29"/>
     </row>
-    <row r="115" spans="25:28" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="115" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y115" s="29"/>
-      <c r="Z115" s="30"/>
+      <c r="Z115" s="29"/>
       <c r="AA115" s="29"/>
       <c r="AB115" s="29"/>
     </row>
@@ -9419,12 +9579,6 @@
       <c r="Z116" s="29"/>
       <c r="AA116" s="29"/>
       <c r="AB116" s="29"/>
-    </row>
-    <row r="117" spans="25:28" x14ac:dyDescent="0.25">
-      <c r="Y117" s="29"/>
-      <c r="Z117" s="29"/>
-      <c r="AA117" s="29"/>
-      <c r="AB117" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Y91" xr:uid="{9EE4866E-E834-4DB8-9ED6-70561D41353B}"/>

</xml_diff>